<commit_message>
20220517 CRE21-022 Update RVP report
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/eHSD0004-RVP Claim_Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/eHSD0004-RVP Claim_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2020\CRE20-0XX (Immu record)\Front-end (Phase X - RVP Report)\ExcelGenerator\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ehp9-fs1\ehs$\Development\InternalChangeControl\2022\CRE21-022 (eHSD0004 COVID19 void records)\Front-end\ExcelGenerator\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,15 +17,16 @@
     <sheet name="02" sheetId="22" r:id="rId3"/>
     <sheet name="03" sheetId="29" r:id="rId4"/>
     <sheet name="04" sheetId="23" r:id="rId5"/>
-    <sheet name="Remark" sheetId="6" r:id="rId6"/>
-    <sheet name="Change History" sheetId="25" r:id="rId7"/>
+    <sheet name="05" sheetId="30" r:id="rId6"/>
+    <sheet name="Remark" sheetId="6" r:id="rId7"/>
+    <sheet name="Change History" sheetId="25" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="137">
   <si>
     <t/>
   </si>
@@ -418,6 +419,58 @@
   </si>
   <si>
     <t>OW</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>eHS(S)D0004-05</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CRE21-022</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>To include COVID-19 vaccination records of “Void” status in RVP reports</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invalidation Status</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invalidated By</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invalidation Reason</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Raw Data of RVP transactions (Voided)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Voided By</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Void Time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Void Reason</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reject Time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rejected By</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invalidation Time</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -430,7 +483,7 @@
     <numFmt numFmtId="177" formatCode="0_ "/>
     <numFmt numFmtId="178" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="新細明體"/>
@@ -525,7 +578,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -851,6 +904,24 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1162,11 +1233,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.625" style="19" customWidth="1"/>
     <col min="2" max="3" width="9" style="19"/>
@@ -1174,7 +1245,7 @@
     <col min="5" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
         <v>69</v>
       </c>
@@ -1182,7 +1253,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
         <v>18</v>
       </c>
@@ -1190,7 +1261,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
         <v>19</v>
       </c>
@@ -1198,7 +1269,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
         <v>20</v>
       </c>
@@ -1206,7 +1277,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
         <v>66</v>
       </c>
@@ -1214,19 +1285,27 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A6" s="49"/>
-      <c r="B6" s="49"/>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="49" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="49"/>
       <c r="B7" s="49"/>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A8" s="48" t="s">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="49"/>
+      <c r="B8" s="49"/>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="49"/>
+      <c r="B9" s="49"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1245,7 +1324,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.75" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.375" style="1" customWidth="1"/>
@@ -1262,7 +1341,7 @@
     <col min="22" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1">
+    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="str">
         <f>Content!A2 &amp; ": " &amp; Content!B2</f>
         <v>eHS(S)D0004-01: Report on eHealth (Subsidies) Accounts with RVP claim transactions by document type</v>
@@ -1283,7 +1362,7 @@
       <c r="P1" s="35"/>
       <c r="Q1" s="35"/>
     </row>
-    <row r="2" spans="1:17" ht="15.75" customHeight="1">
+    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="45"/>
       <c r="C2" s="46"/>
       <c r="D2" s="35"/>
@@ -1301,7 +1380,7 @@
       <c r="P2" s="37"/>
       <c r="Q2" s="37"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" customHeight="1">
+    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
         <v>67</v>
       </c>
@@ -1321,7 +1400,7 @@
       <c r="P3" s="36"/>
       <c r="Q3" s="36"/>
     </row>
-    <row r="4" spans="1:17" ht="15.75" customHeight="1">
+    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="47"/>
       <c r="C4" s="46"/>
       <c r="D4" s="35"/>
@@ -1339,7 +1418,7 @@
       <c r="P4" s="36"/>
       <c r="Q4" s="36"/>
     </row>
-    <row r="5" spans="1:17" s="75" customFormat="1" ht="15.75" customHeight="1">
+    <row r="5" spans="1:17" s="75" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="74" t="s">
         <v>22</v>
       </c>
@@ -1385,7 +1464,7 @@
       </c>
       <c r="Q5" s="76"/>
     </row>
-    <row r="6" spans="1:17" ht="15.75" customHeight="1">
+    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="73" t="s">
         <v>85</v>
       </c>
@@ -1434,7 +1513,7 @@
       </c>
       <c r="Q6" s="35"/>
     </row>
-    <row r="7" spans="1:17" ht="15.75" customHeight="1">
+    <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="73" t="s">
         <v>86</v>
       </c>
@@ -1481,7 +1560,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75" customHeight="1">
+    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="73" t="s">
         <v>21</v>
       </c>
@@ -1530,7 +1609,7 @@
       </c>
       <c r="Q8" s="35"/>
     </row>
-    <row r="9" spans="1:17" ht="15.75" customHeight="1">
+    <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="38"/>
       <c r="C9" s="39"/>
       <c r="D9" s="38"/>
@@ -1548,7 +1627,7 @@
       <c r="P9" s="38"/>
       <c r="Q9" s="38"/>
     </row>
-    <row r="10" spans="1:17" ht="15.75" customHeight="1">
+    <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="35"/>
       <c r="C10" s="35"/>
       <c r="D10" s="35"/>
@@ -1566,7 +1645,7 @@
       <c r="P10" s="38"/>
       <c r="Q10" s="38"/>
     </row>
-    <row r="11" spans="1:17" ht="15.75" customHeight="1">
+    <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="43"/>
       <c r="C11" s="35"/>
       <c r="D11" s="35"/>
@@ -1584,7 +1663,7 @@
       <c r="P11" s="38"/>
       <c r="Q11" s="38"/>
     </row>
-    <row r="12" spans="1:17" ht="15.75" customHeight="1">
+    <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="44"/>
       <c r="C12" s="35"/>
       <c r="D12" s="35"/>
@@ -1602,7 +1681,7 @@
       <c r="P12" s="38"/>
       <c r="Q12" s="38"/>
     </row>
-    <row r="13" spans="1:17" ht="15.75" customHeight="1">
+    <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="44"/>
       <c r="C13" s="35"/>
       <c r="D13" s="35"/>
@@ -1620,7 +1699,7 @@
       <c r="P13" s="35"/>
       <c r="Q13" s="35"/>
     </row>
-    <row r="14" spans="1:17" ht="15.75" customHeight="1">
+    <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="44"/>
       <c r="C14" s="35"/>
       <c r="D14" s="35"/>
@@ -1638,7 +1717,7 @@
       <c r="P14" s="35"/>
       <c r="Q14" s="35"/>
     </row>
-    <row r="15" spans="1:17" ht="15.75" customHeight="1">
+    <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="44"/>
       <c r="C15" s="35"/>
       <c r="D15" s="35"/>
@@ -1656,10 +1735,10 @@
       <c r="P15" s="35"/>
       <c r="Q15" s="35"/>
     </row>
-    <row r="16" spans="1:17" ht="15.75" customHeight="1">
+    <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="44"/>
     </row>
-    <row r="17" spans="2:2" ht="15.75" customHeight="1">
+    <row r="17" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="44"/>
     </row>
   </sheetData>
@@ -1679,7 +1758,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="4" width="14.875" style="1" customWidth="1"/>
@@ -1691,7 +1770,7 @@
     <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="92" t="str">
         <f>Content!A3 &amp; ": " &amp; Content!B3</f>
         <v>eHS(S)D0004-02: Report on yearly RVP transaction (YYYY/YY)</v>
@@ -1710,7 +1789,7 @@
       <c r="M1" s="82"/>
       <c r="N1" s="82"/>
     </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1">
+    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="92"/>
       <c r="B2" s="93"/>
       <c r="C2" s="101"/>
@@ -1726,7 +1805,7 @@
       <c r="M2" s="82"/>
       <c r="N2" s="82"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="94" t="s">
         <v>75</v>
       </c>
@@ -1744,7 +1823,7 @@
       <c r="M3" s="82"/>
       <c r="N3" s="82"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="86"/>
       <c r="B4" s="82"/>
       <c r="C4" s="82"/>
@@ -1760,7 +1839,7 @@
       <c r="M4" s="82"/>
       <c r="N4" s="82"/>
     </row>
-    <row r="5" spans="1:14" ht="15.75" customHeight="1">
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="91" t="s">
         <v>112</v>
       </c>
@@ -1778,7 +1857,7 @@
       <c r="M5" s="82"/>
       <c r="N5" s="82"/>
     </row>
-    <row r="7" spans="1:14" s="23" customFormat="1" ht="47.25" customHeight="1">
+    <row r="7" spans="1:14" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="100"/>
       <c r="B7" s="99" t="s">
         <v>105</v>
@@ -1808,7 +1887,7 @@
       <c r="M7" s="100"/>
       <c r="N7" s="99"/>
     </row>
-    <row r="8" spans="1:14" s="4" customFormat="1" ht="15.75" customHeight="1">
+    <row r="8" spans="1:14" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="88" t="s">
         <v>32</v>
       </c>
@@ -1838,7 +1917,7 @@
       <c r="M8" s="85"/>
       <c r="N8" s="98"/>
     </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1">
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="88" t="s">
         <v>33</v>
       </c>
@@ -1868,7 +1947,7 @@
       <c r="M9" s="82"/>
       <c r="N9" s="82"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1">
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="88" t="s">
         <v>93</v>
       </c>
@@ -1898,7 +1977,7 @@
       <c r="M10" s="82"/>
       <c r="N10" s="82"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1">
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="88" t="s">
         <v>34</v>
       </c>
@@ -1928,7 +2007,7 @@
       <c r="M11" s="82"/>
       <c r="N11" s="82"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1">
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="83" t="s">
         <v>21</v>
       </c>
@@ -1960,7 +2039,7 @@
       <c r="M12" s="82"/>
       <c r="N12" s="82"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" customHeight="1">
+    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="91"/>
       <c r="B13" s="82"/>
       <c r="C13" s="82"/>
@@ -1976,7 +2055,7 @@
       <c r="M13" s="82"/>
       <c r="N13" s="82"/>
     </row>
-    <row r="14" spans="1:14" s="15" customFormat="1" ht="15.75" customHeight="1">
+    <row r="14" spans="1:14" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="91" t="s">
         <v>81</v>
       </c>
@@ -1994,7 +2073,7 @@
       <c r="M14" s="95"/>
       <c r="N14" s="95"/>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="88"/>
       <c r="B15" s="97"/>
       <c r="C15" s="97"/>
@@ -2010,7 +2089,7 @@
       <c r="M15" s="82"/>
       <c r="N15" s="82"/>
     </row>
-    <row r="16" spans="1:14" ht="31.5">
+    <row r="16" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="88"/>
       <c r="B16" s="97" t="s">
         <v>35</v>
@@ -2036,7 +2115,7 @@
       <c r="M16" s="82"/>
       <c r="N16" s="82"/>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="88" t="s">
         <v>32</v>
       </c>
@@ -2056,7 +2135,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="88" t="s">
         <v>33</v>
       </c>
@@ -2076,7 +2155,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="88" t="s">
         <v>93</v>
       </c>
@@ -2096,7 +2175,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="83" t="s">
         <v>34</v>
       </c>
@@ -2116,7 +2195,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="86" t="s">
         <v>21</v>
       </c>
@@ -2136,7 +2215,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="88"/>
       <c r="B22" s="96"/>
       <c r="C22" s="96"/>
@@ -2144,7 +2223,7 @@
       <c r="E22" s="83"/>
       <c r="F22" s="82"/>
     </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="91" t="s">
         <v>111</v>
       </c>
@@ -2154,7 +2233,7 @@
       <c r="E23" s="98"/>
       <c r="F23" s="82"/>
     </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1">
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="88"/>
       <c r="B24" s="98"/>
       <c r="C24" s="98"/>
@@ -2162,7 +2241,7 @@
       <c r="E24" s="98"/>
       <c r="F24" s="82"/>
     </row>
-    <row r="25" spans="1:6" ht="31.5">
+    <row r="25" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="88"/>
       <c r="B25" s="97" t="s">
         <v>35</v>
@@ -2180,7 +2259,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1">
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="88" t="s">
         <v>32</v>
       </c>
@@ -2200,7 +2279,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1">
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="88" t="s">
         <v>33</v>
       </c>
@@ -2220,7 +2299,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1">
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="88" t="s">
         <v>93</v>
       </c>
@@ -2240,7 +2319,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1">
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="83" t="s">
         <v>34</v>
       </c>
@@ -2260,7 +2339,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1">
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="86" t="s">
         <v>21</v>
       </c>
@@ -2280,7 +2359,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1">
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="88"/>
       <c r="B31" s="98"/>
       <c r="C31" s="98"/>
@@ -2288,7 +2367,7 @@
       <c r="E31" s="98"/>
       <c r="F31" s="84"/>
     </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1">
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="91" t="s">
         <v>82</v>
       </c>
@@ -2298,7 +2377,7 @@
       <c r="E32" s="98"/>
       <c r="F32" s="82"/>
     </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1">
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="91"/>
       <c r="B34" s="105" t="s">
         <v>39</v>
@@ -2313,7 +2392,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1">
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="88" t="s">
         <v>32</v>
       </c>
@@ -2330,7 +2409,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="88" t="s">
         <v>33</v>
       </c>
@@ -2347,7 +2426,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="88" t="s">
         <v>93</v>
       </c>
@@ -2364,7 +2443,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="83" t="s">
         <v>34</v>
       </c>
@@ -2381,7 +2460,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1">
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="86" t="s">
         <v>21</v>
       </c>
@@ -2398,14 +2477,14 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1">
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="88"/>
       <c r="B40" s="98"/>
       <c r="C40" s="98"/>
       <c r="D40" s="98"/>
       <c r="E40" s="98"/>
     </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1">
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="91" t="s">
         <v>89</v>
       </c>
@@ -2414,7 +2493,7 @@
       <c r="D41" s="82"/>
       <c r="E41" s="82"/>
     </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="82"/>
       <c r="B43" s="105" t="s">
         <v>39</v>
@@ -2429,7 +2508,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="88" t="s">
         <v>32</v>
       </c>
@@ -2446,7 +2525,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="88" t="s">
         <v>33</v>
       </c>
@@ -2463,7 +2542,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1">
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="88" t="s">
         <v>93</v>
       </c>
@@ -2480,7 +2559,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1">
+    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="83" t="s">
         <v>34</v>
       </c>
@@ -2497,7 +2576,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="86" t="s">
         <v>21</v>
       </c>
@@ -2514,7 +2593,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1">
+    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="91" t="s">
         <v>83</v>
       </c>
@@ -2523,7 +2602,7 @@
       <c r="D50" s="82"/>
       <c r="E50" s="82"/>
     </row>
-    <row r="52" spans="1:5" ht="66.75" customHeight="1">
+    <row r="52" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="82"/>
       <c r="B52" s="102" t="s">
         <v>42</v>
@@ -2538,7 +2617,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1">
+    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="88" t="s">
         <v>32</v>
       </c>
@@ -2555,7 +2634,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1">
+    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="88" t="s">
         <v>33</v>
       </c>
@@ -2572,7 +2651,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15.75" customHeight="1">
+    <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="88" t="s">
         <v>93</v>
       </c>
@@ -2589,7 +2668,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15.75" customHeight="1">
+    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="83" t="s">
         <v>34</v>
       </c>
@@ -2606,7 +2685,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="15.75" customHeight="1">
+    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="86" t="s">
         <v>21</v>
       </c>
@@ -2623,7 +2702,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15.75" customHeight="1">
+    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="91" t="s">
         <v>90</v>
       </c>
@@ -2632,7 +2711,7 @@
       <c r="D59" s="82"/>
       <c r="E59" s="82"/>
     </row>
-    <row r="61" spans="1:5" ht="71.25" customHeight="1">
+    <row r="61" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="82"/>
       <c r="B61" s="102" t="s">
         <v>42</v>
@@ -2647,7 +2726,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="88" t="s">
         <v>32</v>
       </c>
@@ -2664,7 +2743,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1">
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="88" t="s">
         <v>33</v>
       </c>
@@ -2681,7 +2760,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1">
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="88" t="s">
         <v>93</v>
       </c>
@@ -2698,7 +2777,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="15.75" customHeight="1">
+    <row r="65" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="83" t="s">
         <v>34</v>
       </c>
@@ -2717,7 +2796,7 @@
       <c r="F65" s="82"/>
       <c r="G65" s="82"/>
     </row>
-    <row r="66" spans="1:16" ht="15.75" customHeight="1">
+    <row r="66" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="86" t="s">
         <v>21</v>
       </c>
@@ -2736,14 +2815,14 @@
       <c r="F66" s="82"/>
       <c r="G66" s="82"/>
     </row>
-    <row r="67" spans="1:16" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="67" spans="1:16" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="86"/>
       <c r="B67" s="98"/>
       <c r="C67" s="98"/>
       <c r="D67" s="98"/>
       <c r="E67" s="98"/>
     </row>
-    <row r="68" spans="1:16" ht="15.75" customHeight="1">
+    <row r="68" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="91" t="s">
         <v>115</v>
       </c>
@@ -2763,7 +2842,7 @@
       <c r="O68" s="82"/>
       <c r="P68" s="82"/>
     </row>
-    <row r="69" spans="1:16" ht="15.75" customHeight="1">
+    <row r="69" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="86"/>
       <c r="B69" s="98"/>
       <c r="C69" s="98"/>
@@ -2781,7 +2860,7 @@
       <c r="O69" s="82"/>
       <c r="P69" s="82"/>
     </row>
-    <row r="70" spans="1:16" ht="31.5" customHeight="1">
+    <row r="70" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="86"/>
       <c r="B70" s="102" t="s">
         <v>45</v>
@@ -2804,7 +2883,7 @@
       <c r="J70" s="82"/>
       <c r="K70" s="82"/>
     </row>
-    <row r="71" spans="1:16" ht="15.75" customHeight="1">
+    <row r="71" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="86" t="s">
         <v>32</v>
       </c>
@@ -2827,7 +2906,7 @@
       <c r="J71" s="82"/>
       <c r="K71" s="82"/>
     </row>
-    <row r="72" spans="1:16" ht="15.75" customHeight="1">
+    <row r="72" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="86" t="s">
         <v>32</v>
       </c>
@@ -2850,7 +2929,7 @@
       <c r="J72" s="82"/>
       <c r="K72" s="82"/>
     </row>
-    <row r="73" spans="1:16" ht="15.75" customHeight="1">
+    <row r="73" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="86" t="s">
         <v>93</v>
       </c>
@@ -2873,7 +2952,7 @@
       <c r="J73" s="82"/>
       <c r="K73" s="82"/>
     </row>
-    <row r="74" spans="1:16" ht="15.75" customHeight="1">
+    <row r="74" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="86" t="s">
         <v>34</v>
       </c>
@@ -2896,7 +2975,7 @@
       <c r="J74" s="82"/>
       <c r="K74" s="82"/>
     </row>
-    <row r="75" spans="1:16" ht="15.75" customHeight="1">
+    <row r="75" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="83" t="s">
         <v>21</v>
       </c>
@@ -2921,13 +3000,13 @@
       <c r="J75" s="82"/>
       <c r="K75" s="82"/>
     </row>
-    <row r="77" spans="1:16" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="77" spans="1:16" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="91" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="78" spans="1:16" s="82" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="79" spans="1:16" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="78" spans="1:16" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:16" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="105" t="s">
         <v>39</v>
       </c>
@@ -2938,7 +3017,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:16" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="80" spans="1:16" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="88" t="s">
         <v>32</v>
       </c>
@@ -2952,7 +3031,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="81" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="81" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="88" t="s">
         <v>33</v>
       </c>
@@ -2966,7 +3045,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="82" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="82" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="88" t="s">
         <v>93</v>
       </c>
@@ -2980,7 +3059,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="83" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="83" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="83" t="s">
         <v>34</v>
       </c>
@@ -2994,7 +3073,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="84" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="84" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="86" t="s">
         <v>21</v>
       </c>
@@ -3008,14 +3087,14 @@
         <v>68</v>
       </c>
     </row>
-    <row r="85" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="86" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="85" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="91" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="87" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="88" spans="1:7" s="82" customFormat="1" ht="68.25" customHeight="1">
+    <row r="87" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" spans="1:7" s="82" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="102" t="s">
         <v>42</v>
       </c>
@@ -3029,7 +3108,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="89" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="89" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="88" t="s">
         <v>32</v>
       </c>
@@ -3046,7 +3125,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="90" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="90" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="88" t="s">
         <v>33</v>
       </c>
@@ -3063,7 +3142,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="91" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="91" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="88" t="s">
         <v>93</v>
       </c>
@@ -3080,7 +3159,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="92" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="92" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="83" t="s">
         <v>34</v>
       </c>
@@ -3097,7 +3176,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="93" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="93" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="86" t="s">
         <v>21</v>
       </c>
@@ -3114,14 +3193,14 @@
         <v>68</v>
       </c>
     </row>
-    <row r="94" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="94" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="86"/>
       <c r="B94" s="98"/>
       <c r="C94" s="98"/>
       <c r="D94" s="98"/>
       <c r="E94" s="98"/>
     </row>
-    <row r="95" spans="1:7" ht="15.75" customHeight="1">
+    <row r="95" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="91" t="s">
         <v>116</v>
       </c>
@@ -3132,7 +3211,7 @@
       <c r="F95" s="82"/>
       <c r="G95" s="82"/>
     </row>
-    <row r="97" spans="1:16" ht="31.5">
+    <row r="97" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A97" s="82"/>
       <c r="B97" s="102" t="s">
         <v>45</v>
@@ -3151,7 +3230,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="98" spans="1:16" ht="15.75" customHeight="1">
+    <row r="98" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="88" t="s">
         <v>32</v>
       </c>
@@ -3170,7 +3249,7 @@
       <c r="F98" s="82"/>
       <c r="G98" s="85"/>
     </row>
-    <row r="99" spans="1:16" ht="15.75" customHeight="1">
+    <row r="99" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="88" t="s">
         <v>33</v>
       </c>
@@ -3189,7 +3268,7 @@
       <c r="F99" s="82"/>
       <c r="G99" s="82"/>
     </row>
-    <row r="100" spans="1:16" ht="15.75" customHeight="1">
+    <row r="100" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="88" t="s">
         <v>93</v>
       </c>
@@ -3208,7 +3287,7 @@
       <c r="F100" s="82"/>
       <c r="G100" s="82"/>
     </row>
-    <row r="101" spans="1:16" ht="15.75" customHeight="1">
+    <row r="101" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="83" t="s">
         <v>34</v>
       </c>
@@ -3227,7 +3306,7 @@
       <c r="F101" s="82"/>
       <c r="G101" s="82"/>
     </row>
-    <row r="102" spans="1:16" ht="15.75" customHeight="1">
+    <row r="102" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="86" t="s">
         <v>21</v>
       </c>
@@ -3248,7 +3327,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="103" spans="1:16" ht="15.75" customHeight="1">
+    <row r="103" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="86"/>
       <c r="B103" s="96"/>
       <c r="C103" s="96"/>
@@ -3257,7 +3336,7 @@
       <c r="F103" s="82"/>
       <c r="G103" s="82"/>
     </row>
-    <row r="104" spans="1:16" ht="15.75" customHeight="1">
+    <row r="104" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="91" t="s">
         <v>117</v>
       </c>
@@ -3268,7 +3347,7 @@
       <c r="F104" s="82"/>
       <c r="G104" s="82"/>
     </row>
-    <row r="106" spans="1:16" ht="31.5">
+    <row r="106" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A106" s="82"/>
       <c r="B106" s="102" t="s">
         <v>45</v>
@@ -3287,7 +3366,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="107" spans="1:16" ht="15.75" customHeight="1">
+    <row r="107" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="88" t="s">
         <v>32</v>
       </c>
@@ -3306,7 +3385,7 @@
       <c r="F107" s="82"/>
       <c r="G107" s="85"/>
     </row>
-    <row r="108" spans="1:16" ht="15.75" customHeight="1">
+    <row r="108" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="88" t="s">
         <v>33</v>
       </c>
@@ -3334,7 +3413,7 @@
       <c r="O108" s="82"/>
       <c r="P108" s="82"/>
     </row>
-    <row r="109" spans="1:16" ht="15.75" customHeight="1">
+    <row r="109" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="88" t="s">
         <v>93</v>
       </c>
@@ -3362,7 +3441,7 @@
       <c r="O109" s="82"/>
       <c r="P109" s="82"/>
     </row>
-    <row r="110" spans="1:16" ht="15.75" customHeight="1">
+    <row r="110" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="83" t="s">
         <v>34</v>
       </c>
@@ -3390,7 +3469,7 @@
       <c r="O110" s="82"/>
       <c r="P110" s="82"/>
     </row>
-    <row r="111" spans="1:16" ht="15.75" customHeight="1">
+    <row r="111" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="86" t="s">
         <v>21</v>
       </c>
@@ -3420,7 +3499,7 @@
       <c r="O111" s="82"/>
       <c r="P111" s="82"/>
     </row>
-    <row r="112" spans="1:16" ht="15.75" customHeight="1">
+    <row r="112" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="86"/>
       <c r="B112" s="98"/>
       <c r="C112" s="98"/>
@@ -3438,13 +3517,13 @@
       <c r="O112" s="82"/>
       <c r="P112" s="82"/>
     </row>
-    <row r="113" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="113" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="108" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="114" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="115" spans="1:7" s="82" customFormat="1" ht="44.25" customHeight="1">
+    <row r="114" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="1:7" s="82" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="52" t="s">
         <v>45</v>
       </c>
@@ -3461,7 +3540,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="116" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="116" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="83" t="s">
         <v>32</v>
       </c>
@@ -3478,7 +3557,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="117" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="117" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="83" t="s">
         <v>33</v>
       </c>
@@ -3495,7 +3574,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="118" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="118" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="83" t="s">
         <v>93</v>
       </c>
@@ -3512,7 +3591,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="119" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="119" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="83" t="s">
         <v>34</v>
       </c>
@@ -3529,7 +3608,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="120" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="120" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="83" t="s">
         <v>21</v>
       </c>
@@ -3549,14 +3628,14 @@
         <v>68</v>
       </c>
     </row>
-    <row r="121" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="121" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" s="98"/>
       <c r="C121" s="98"/>
       <c r="D121" s="98"/>
       <c r="E121" s="98"/>
       <c r="G121" s="98"/>
     </row>
-    <row r="122" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="122" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="108" t="s">
         <v>101</v>
       </c>
@@ -3566,14 +3645,14 @@
       <c r="E122" s="98"/>
       <c r="G122" s="98"/>
     </row>
-    <row r="123" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="123" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" s="98"/>
       <c r="C123" s="98"/>
       <c r="D123" s="98"/>
       <c r="E123" s="98"/>
       <c r="G123" s="98"/>
     </row>
-    <row r="124" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="124" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" s="105" t="s">
         <v>39</v>
       </c>
@@ -3586,7 +3665,7 @@
       <c r="E124" s="98"/>
       <c r="G124" s="98"/>
     </row>
-    <row r="125" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="125" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="83" t="s">
         <v>32</v>
       </c>
@@ -3602,7 +3681,7 @@
       <c r="E125" s="98"/>
       <c r="G125" s="98"/>
     </row>
-    <row r="126" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="126" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="83" t="s">
         <v>33</v>
       </c>
@@ -3618,7 +3697,7 @@
       <c r="E126" s="98"/>
       <c r="G126" s="98"/>
     </row>
-    <row r="127" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="127" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="83" t="s">
         <v>93</v>
       </c>
@@ -3634,7 +3713,7 @@
       <c r="E127" s="98"/>
       <c r="G127" s="98"/>
     </row>
-    <row r="128" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="128" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="83" t="s">
         <v>34</v>
       </c>
@@ -3650,7 +3729,7 @@
       <c r="E128" s="98"/>
       <c r="G128" s="98"/>
     </row>
-    <row r="129" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="129" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="83" t="s">
         <v>21</v>
       </c>
@@ -3666,14 +3745,14 @@
       <c r="E129" s="98"/>
       <c r="G129" s="98"/>
     </row>
-    <row r="130" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="130" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B130" s="98"/>
       <c r="C130" s="98"/>
       <c r="D130" s="98"/>
       <c r="E130" s="98"/>
       <c r="G130" s="98"/>
     </row>
-    <row r="131" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="131" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="108" t="s">
         <v>102</v>
       </c>
@@ -3683,14 +3762,14 @@
       <c r="E131" s="98"/>
       <c r="G131" s="98"/>
     </row>
-    <row r="132" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="132" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="98"/>
       <c r="C132" s="98"/>
       <c r="D132" s="98"/>
       <c r="E132" s="98"/>
       <c r="G132" s="98"/>
     </row>
-    <row r="133" spans="1:7" s="82" customFormat="1" ht="64.5" customHeight="1">
+    <row r="133" spans="1:7" s="82" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" s="97" t="s">
         <v>104</v>
       </c>
@@ -3705,7 +3784,7 @@
       </c>
       <c r="G133" s="98"/>
     </row>
-    <row r="134" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="134" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="83" t="s">
         <v>32</v>
       </c>
@@ -3723,7 +3802,7 @@
       </c>
       <c r="G134" s="98"/>
     </row>
-    <row r="135" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="135" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="83" t="s">
         <v>33</v>
       </c>
@@ -3741,7 +3820,7 @@
       </c>
       <c r="G135" s="98"/>
     </row>
-    <row r="136" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="136" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="83" t="s">
         <v>93</v>
       </c>
@@ -3759,7 +3838,7 @@
       </c>
       <c r="G136" s="98"/>
     </row>
-    <row r="137" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="137" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="83" t="s">
         <v>34</v>
       </c>
@@ -3777,7 +3856,7 @@
       </c>
       <c r="G137" s="98"/>
     </row>
-    <row r="138" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="138" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="83" t="s">
         <v>21</v>
       </c>
@@ -3794,13 +3873,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="140" spans="1:7" ht="15.75" customHeight="1">
+    <row r="139" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="83" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="15.75" customHeight="1">
+    <row r="141" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="106" t="s">
         <v>118</v>
       </c>
@@ -3822,7 +3901,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="14.875" style="1" customWidth="1"/>
@@ -3836,7 +3915,7 @@
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="str">
         <f>Content!A4 &amp; ": " &amp; Content!B4</f>
         <v>eHS(S)D0004-03: Report on RVP transaction (by cutoff date)</v>
@@ -3846,14 +3925,14 @@
       <c r="D1" s="9"/>
       <c r="E1" s="13"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12"/>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
       <c r="D2" s="9"/>
       <c r="E2" s="13"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>75</v>
       </c>
@@ -3862,14 +3941,14 @@
       <c r="D3" s="9"/>
       <c r="E3" s="13"/>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
       <c r="D4" s="9"/>
       <c r="E4" s="13"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>77</v>
       </c>
@@ -3878,15 +3957,15 @@
       <c r="D5" s="9"/>
       <c r="E5" s="13"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="23" customFormat="1">
+    <row r="8" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="29" t="s">
         <v>45</v>
       </c>
@@ -3905,7 +3984,7 @@
       <c r="H8" s="22"/>
       <c r="J8" s="22"/>
     </row>
-    <row r="9" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1">
+    <row r="9" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>32</v>
       </c>
@@ -3924,7 +4003,7 @@
       <c r="H9" s="6"/>
       <c r="J9" s="21"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>33</v>
       </c>
@@ -3942,7 +4021,7 @@
       </c>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:10" s="78" customFormat="1" ht="15.75" customHeight="1">
+    <row r="11" spans="1:10" s="78" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="83" t="s">
         <v>93</v>
       </c>
@@ -3961,7 +4040,7 @@
       <c r="F11" s="77"/>
       <c r="H11" s="79"/>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>34</v>
       </c>
@@ -3978,7 +4057,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -3998,19 +4077,19 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="20"/>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>78</v>
       </c>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:10" s="23" customFormat="1">
+    <row r="16" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="29" t="s">
         <v>45</v>
       </c>
@@ -4029,7 +4108,7 @@
       <c r="H16" s="22"/>
       <c r="J16" s="22"/>
     </row>
-    <row r="17" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1">
+    <row r="17" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>32</v>
       </c>
@@ -4049,7 +4128,7 @@
       <c r="H17" s="6"/>
       <c r="J17" s="21"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>33</v>
       </c>
@@ -4068,7 +4147,7 @@
       <c r="G18" s="20"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:10" s="78" customFormat="1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:10" s="78" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="83" t="s">
         <v>93</v>
       </c>
@@ -4088,7 +4167,7 @@
       <c r="G19" s="80"/>
       <c r="H19" s="79"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>34</v>
       </c>
@@ -4106,7 +4185,7 @@
       </c>
       <c r="G20" s="20"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -4126,7 +4205,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="22" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="83"/>
       <c r="B22" s="98"/>
       <c r="C22" s="98"/>
@@ -4135,7 +4214,7 @@
       <c r="F22" s="81"/>
       <c r="G22" s="98"/>
     </row>
-    <row r="23" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="23" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="83" t="s">
         <v>94</v>
       </c>
@@ -4146,7 +4225,7 @@
       <c r="F23" s="81"/>
       <c r="G23" s="98"/>
     </row>
-    <row r="24" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="24" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="83"/>
       <c r="B24" s="102" t="s">
         <v>45</v>
@@ -4165,7 +4244,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="25" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="83" t="s">
         <v>32</v>
       </c>
@@ -4184,7 +4263,7 @@
       <c r="F25" s="98"/>
       <c r="G25" s="98"/>
     </row>
-    <row r="26" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="26" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="83" t="s">
         <v>33</v>
       </c>
@@ -4203,7 +4282,7 @@
       <c r="F26" s="98"/>
       <c r="G26" s="98"/>
     </row>
-    <row r="27" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="27" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="83" t="s">
         <v>93</v>
       </c>
@@ -4222,7 +4301,7 @@
       <c r="F27" s="98"/>
       <c r="G27" s="98"/>
     </row>
-    <row r="28" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="28" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="83" t="s">
         <v>34</v>
       </c>
@@ -4241,7 +4320,7 @@
       <c r="F28" s="98"/>
       <c r="G28" s="98"/>
     </row>
-    <row r="29" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="29" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="83" t="s">
         <v>21</v>
       </c>
@@ -4262,14 +4341,14 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
       <c r="D30" s="20"/>
       <c r="E30" s="20"/>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
         <v>79</v>
       </c>
@@ -4278,15 +4357,15 @@
       <c r="D31" s="20"/>
       <c r="E31" s="20"/>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="23" customFormat="1">
+    <row r="34" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="29" t="s">
         <v>45</v>
       </c>
@@ -4305,7 +4384,7 @@
       <c r="H34" s="22"/>
       <c r="J34" s="22"/>
     </row>
-    <row r="35" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1">
+    <row r="35" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>32</v>
       </c>
@@ -4324,7 +4403,7 @@
       <c r="H35" s="6"/>
       <c r="J35" s="21"/>
     </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1">
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>33</v>
       </c>
@@ -4342,7 +4421,7 @@
       </c>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="37" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="83" t="s">
         <v>93</v>
       </c>
@@ -4361,7 +4440,7 @@
       <c r="F37" s="81"/>
       <c r="H37" s="83"/>
     </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1">
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>34</v>
       </c>
@@ -4378,7 +4457,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1">
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>21</v>
       </c>
@@ -4398,19 +4477,19 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1">
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="20"/>
       <c r="C40" s="20"/>
       <c r="D40" s="20"/>
     </row>
-    <row r="41" spans="1:10" ht="15.75" customHeight="1">
+    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>65</v>
       </c>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="1:10" s="23" customFormat="1">
+    <row r="42" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="29" t="s">
         <v>45</v>
       </c>
@@ -4429,7 +4508,7 @@
       <c r="H42" s="22"/>
       <c r="J42" s="22"/>
     </row>
-    <row r="43" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1">
+    <row r="43" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>32</v>
       </c>
@@ -4449,7 +4528,7 @@
       <c r="H43" s="6"/>
       <c r="J43" s="21"/>
     </row>
-    <row r="44" spans="1:10" ht="15.75" customHeight="1">
+    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>33</v>
       </c>
@@ -4468,7 +4547,7 @@
       <c r="G44" s="20"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="45" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="83" t="s">
         <v>93</v>
       </c>
@@ -4488,7 +4567,7 @@
       <c r="G45" s="96"/>
       <c r="H45" s="83"/>
     </row>
-    <row r="46" spans="1:10" ht="15.75" customHeight="1">
+    <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>34</v>
       </c>
@@ -4506,7 +4585,7 @@
       </c>
       <c r="G46" s="20"/>
     </row>
-    <row r="47" spans="1:10" ht="15.75" customHeight="1">
+    <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>21</v>
       </c>
@@ -4526,7 +4605,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="48" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="83"/>
       <c r="B48" s="98"/>
       <c r="C48" s="98"/>
@@ -4535,7 +4614,7 @@
       <c r="F48" s="81"/>
       <c r="G48" s="98"/>
     </row>
-    <row r="49" spans="1:10" ht="15.75" customHeight="1">
+    <row r="49" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="83" t="s">
         <v>95</v>
       </c>
@@ -4546,7 +4625,7 @@
       <c r="F49" s="81"/>
       <c r="G49" s="98"/>
     </row>
-    <row r="50" spans="1:10" ht="15.75" customHeight="1">
+    <row r="50" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="83"/>
       <c r="B50" s="102" t="s">
         <v>45</v>
@@ -4565,7 +4644,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15.75" customHeight="1">
+    <row r="51" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="83" t="s">
         <v>32</v>
       </c>
@@ -4584,7 +4663,7 @@
       <c r="F51" s="98"/>
       <c r="G51" s="98"/>
     </row>
-    <row r="52" spans="1:10" s="23" customFormat="1">
+    <row r="52" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="83" t="s">
         <v>33</v>
       </c>
@@ -4605,7 +4684,7 @@
       <c r="H52" s="22"/>
       <c r="J52" s="22"/>
     </row>
-    <row r="53" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1">
+    <row r="53" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="83" t="s">
         <v>93</v>
       </c>
@@ -4626,7 +4705,7 @@
       <c r="H53" s="6"/>
       <c r="J53" s="21"/>
     </row>
-    <row r="54" spans="1:10" ht="15.75" customHeight="1">
+    <row r="54" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="83" t="s">
         <v>34</v>
       </c>
@@ -4646,7 +4725,7 @@
       <c r="G54" s="98"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:10" ht="15.75" customHeight="1">
+    <row r="55" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="83" t="s">
         <v>21</v>
       </c>
@@ -4667,14 +4746,14 @@
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15.75" customHeight="1">
+    <row r="56" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="20"/>
       <c r="C56" s="20"/>
       <c r="D56" s="20"/>
       <c r="E56" s="20"/>
     </row>
-    <row r="57" spans="1:10" ht="15.75" customHeight="1">
+    <row r="57" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="32" t="s">
         <v>80</v>
       </c>
@@ -4683,10 +4762,10 @@
       <c r="D57" s="20"/>
       <c r="E57" s="20"/>
     </row>
-    <row r="58" spans="1:10" ht="15.75" customHeight="1">
+    <row r="58" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
     </row>
-    <row r="59" spans="1:10" s="23" customFormat="1" ht="16.5">
+    <row r="59" spans="1:10" s="23" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>63</v>
       </c>
@@ -4699,7 +4778,7 @@
       <c r="H59" s="22"/>
       <c r="J59" s="22"/>
     </row>
-    <row r="60" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1">
+    <row r="60" spans="1:10" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="23"/>
       <c r="B60" s="29" t="s">
         <v>45</v>
@@ -4720,7 +4799,7 @@
       <c r="H60" s="6"/>
       <c r="J60" s="21"/>
     </row>
-    <row r="61" spans="1:10" ht="15.75" customHeight="1">
+    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>32</v>
       </c>
@@ -4740,7 +4819,7 @@
       <c r="G61" s="4"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:10" ht="15.75" customHeight="1">
+    <row r="62" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>33</v>
       </c>
@@ -4757,7 +4836,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="63" spans="1:10" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="83" t="s">
         <v>93</v>
       </c>
@@ -4776,7 +4855,7 @@
       <c r="F63" s="98"/>
       <c r="G63" s="98"/>
     </row>
-    <row r="64" spans="1:10" ht="15.75" customHeight="1">
+    <row r="64" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>34</v>
       </c>
@@ -4793,7 +4872,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="15.75" customHeight="1">
+    <row r="65" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>21</v>
       </c>
@@ -4813,19 +4892,19 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15.75" customHeight="1">
+    <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="20"/>
       <c r="C66" s="20"/>
       <c r="D66" s="20"/>
     </row>
-    <row r="67" spans="1:7" ht="15.75" customHeight="1">
+    <row r="67" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>65</v>
       </c>
       <c r="G67" s="2"/>
     </row>
-    <row r="68" spans="1:7" ht="15.75" customHeight="1">
+    <row r="68" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="23"/>
       <c r="B68" s="29" t="s">
         <v>45</v>
@@ -4844,7 +4923,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="15.75" customHeight="1">
+    <row r="69" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>32</v>
       </c>
@@ -4863,7 +4942,7 @@
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
     </row>
-    <row r="70" spans="1:7" ht="15.75" customHeight="1">
+    <row r="70" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>33</v>
       </c>
@@ -4880,7 +4959,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1">
+    <row r="71" spans="1:7" s="82" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="83" t="s">
         <v>93</v>
       </c>
@@ -4898,7 +4977,7 @@
       </c>
       <c r="F71" s="81"/>
     </row>
-    <row r="72" spans="1:7" ht="15.75" customHeight="1">
+    <row r="72" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>34</v>
       </c>
@@ -4915,7 +4994,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15.75" customHeight="1">
+    <row r="73" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>21</v>
       </c>
@@ -4935,14 +5014,14 @@
         <v>68</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="15.75" customHeight="1">
+    <row r="74" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="20"/>
       <c r="C74" s="20"/>
       <c r="D74" s="20"/>
       <c r="E74" s="20"/>
     </row>
-    <row r="75" spans="1:7" ht="15.75" customHeight="1">
+    <row r="75" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="83" t="s">
         <v>95</v>
       </c>
@@ -4953,7 +5032,7 @@
       <c r="F75" s="81"/>
       <c r="G75" s="98"/>
     </row>
-    <row r="76" spans="1:7" ht="15.75" customHeight="1">
+    <row r="76" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="83"/>
       <c r="B76" s="102" t="s">
         <v>45</v>
@@ -4972,7 +5051,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="15.75" customHeight="1">
+    <row r="77" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="83" t="s">
         <v>32</v>
       </c>
@@ -4991,7 +5070,7 @@
       <c r="F77" s="98"/>
       <c r="G77" s="98"/>
     </row>
-    <row r="78" spans="1:7" ht="15.75" customHeight="1">
+    <row r="78" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="83" t="s">
         <v>33</v>
       </c>
@@ -5010,7 +5089,7 @@
       <c r="F78" s="98"/>
       <c r="G78" s="98"/>
     </row>
-    <row r="79" spans="1:7" ht="15.75" customHeight="1">
+    <row r="79" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="83" t="s">
         <v>93</v>
       </c>
@@ -5029,7 +5108,7 @@
       <c r="F79" s="98"/>
       <c r="G79" s="98"/>
     </row>
-    <row r="80" spans="1:7" ht="15.75" customHeight="1">
+    <row r="80" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="83" t="s">
         <v>34</v>
       </c>
@@ -5048,7 +5127,7 @@
       <c r="F80" s="98"/>
       <c r="G80" s="98"/>
     </row>
-    <row r="81" spans="1:7" ht="15.75" customHeight="1">
+    <row r="81" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="83" t="s">
         <v>21</v>
       </c>
@@ -5086,7 +5165,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.625" style="17" customWidth="1"/>
     <col min="2" max="2" width="25" style="10" customWidth="1"/>
@@ -5107,7 +5186,7 @@
     <col min="17" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="16" customFormat="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:16" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="str">
         <f>Content!A5 &amp; ": " &amp; Content!B5</f>
         <v xml:space="preserve">eHS(S)D0004-04: Raw Data of RVP transactions </v>
@@ -5130,7 +5209,7 @@
       <c r="O1" s="62"/>
       <c r="P1" s="62"/>
     </row>
-    <row r="2" spans="1:16" ht="15.75" customHeight="1">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="63"/>
       <c r="B2" s="57"/>
       <c r="C2" s="51"/>
@@ -5148,7 +5227,7 @@
       <c r="O2" s="51"/>
       <c r="P2" s="51"/>
     </row>
-    <row r="3" spans="1:16" s="16" customFormat="1" ht="15.75" customHeight="1">
+    <row r="3" spans="1:16" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
         <v>67</v>
       </c>
@@ -5168,7 +5247,7 @@
       <c r="O3" s="62"/>
       <c r="P3" s="62"/>
     </row>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1">
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="51"/>
       <c r="B4" s="51"/>
       <c r="C4" s="51"/>
@@ -5188,7 +5267,7 @@
       <c r="O4" s="51"/>
       <c r="P4" s="51"/>
     </row>
-    <row r="5" spans="1:16" s="3" customFormat="1" ht="15.75" customHeight="1">
+    <row r="5" spans="1:16" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="54" t="s">
         <v>46</v>
       </c>
@@ -5238,7 +5317,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="16.5" customHeight="1"/>
+    <row r="8" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5249,186 +5328,400 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:Y8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.375" style="17" customWidth="1"/>
+    <col min="2" max="2" width="27.125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="11.875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="15" style="70" customWidth="1"/>
+    <col min="5" max="5" width="28.125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="26.125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="17" customWidth="1"/>
+    <col min="8" max="8" width="12.5" style="70" customWidth="1"/>
+    <col min="9" max="9" width="11.25" style="17" customWidth="1"/>
+    <col min="10" max="10" width="10.625" style="17" customWidth="1"/>
+    <col min="11" max="11" width="11.875" style="17" customWidth="1"/>
+    <col min="12" max="12" width="35.625" style="17" customWidth="1"/>
+    <col min="13" max="13" width="31.25" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.875" style="18" customWidth="1"/>
+    <col min="15" max="15" width="11.25" style="17" customWidth="1"/>
+    <col min="16" max="16" width="18.75" style="17" customWidth="1"/>
+    <col min="17" max="17" width="25" style="18" customWidth="1"/>
+    <col min="18" max="18" width="25" style="10" customWidth="1"/>
+    <col min="19" max="19" width="34" style="17" customWidth="1"/>
+    <col min="20" max="20" width="25" style="17" customWidth="1"/>
+    <col min="21" max="21" width="25" style="10" customWidth="1"/>
+    <col min="22" max="22" width="34" style="17" customWidth="1"/>
+    <col min="23" max="23" width="25" style="17" customWidth="1"/>
+    <col min="24" max="24" width="25" style="10" customWidth="1"/>
+    <col min="25" max="25" width="34" style="17" customWidth="1"/>
+    <col min="26" max="16384" width="9" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="62" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="59" t="str">
+        <f>Content!A6 &amp; ": " &amp; Content!B6</f>
+        <v>eHS(S)D0004-05: Raw Data of RVP transactions (Voided)</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="112"/>
+      <c r="R1" s="109"/>
+      <c r="U1" s="109"/>
+      <c r="X1" s="109"/>
+    </row>
+    <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="63"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="113"/>
+      <c r="R2" s="110"/>
+    </row>
+    <row r="3" spans="1:25" s="62" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="58"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="61"/>
+      <c r="Q3" s="112"/>
+      <c r="R3" s="109"/>
+      <c r="U3" s="109"/>
+      <c r="X3" s="109"/>
+    </row>
+    <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="81"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
+      <c r="N4" s="65" t="s">
+        <v>0</v>
+      </c>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="114"/>
+      <c r="R4" s="110"/>
+    </row>
+    <row r="5" spans="1:25" s="52" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="L5" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="M5" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="N5" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="O5" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="P5" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q5" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="R5" s="56" t="s">
+        <v>132</v>
+      </c>
+      <c r="S5" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="T5" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="U5" s="111" t="s">
+        <v>134</v>
+      </c>
+      <c r="V5" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="W5" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="X5" s="111" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y5" s="52" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.25" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="77.125" style="15" customWidth="1"/>
     <col min="3" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="50"/>
       <c r="B1" s="50"/>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="50"/>
       <c r="B2" s="50"/>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="50"/>
       <c r="B3" s="50"/>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50"/>
       <c r="B4" s="50"/>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="50"/>
       <c r="B5" s="50"/>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="50"/>
       <c r="B6" s="50"/>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="50"/>
       <c r="B7" s="50"/>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="50"/>
       <c r="B8" s="50"/>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="50"/>
       <c r="B9" s="50"/>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="50"/>
       <c r="B10" s="50"/>
     </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
     </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
     </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
     </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
     </row>
-    <row r="16" spans="1:2" ht="15.75" customHeight="1">
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
     </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1">
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
     </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1">
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
     </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1">
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
     </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1">
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
     </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1">
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
     </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1">
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
     </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1">
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
     </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1">
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
     </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1">
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
     </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1">
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
     </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1">
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
     </row>
-    <row r="28" spans="1:2" ht="15.75" customHeight="1">
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
     </row>
-    <row r="29" spans="1:2" ht="15.75" customHeight="1">
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
     </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1">
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
     </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1">
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
     </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1">
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
     </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1">
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
     </row>
-    <row r="34" spans="1:2" ht="15.75" customHeight="1">
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
     </row>
-    <row r="35" spans="1:2" ht="15.75" customHeight="1">
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
     </row>
-    <row r="37" spans="1:2" ht="15.75" customHeight="1">
+    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="50"/>
       <c r="B37" s="50"/>
     </row>
-    <row r="38" spans="1:2" ht="15.75" customHeight="1">
+    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="50"/>
       <c r="B38" s="50"/>
     </row>
-    <row r="39" spans="1:2" ht="15.75" customHeight="1">
+    <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="50"/>
       <c r="B39" s="50"/>
     </row>
-    <row r="40" spans="1:2" ht="15.75" customHeight="1">
+    <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="50"/>
       <c r="B40" s="50"/>
     </row>
-    <row r="41" spans="1:2" ht="15.75" customHeight="1">
+    <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="50"/>
       <c r="B41" s="50"/>
     </row>
-    <row r="42" spans="1:2" ht="15.75" customHeight="1">
+    <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="50"/>
       <c r="B42" s="50"/>
     </row>
-    <row r="43" spans="1:2" ht="15.75" customHeight="1">
+    <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="50"/>
       <c r="B43" s="50"/>
     </row>
-    <row r="44" spans="1:2" ht="15.75" customHeight="1">
+    <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="50"/>
       <c r="B44" s="50"/>
     </row>
-    <row r="45" spans="1:2" ht="15.75" customHeight="1">
+    <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="50"/>
       <c r="B45" s="50"/>
     </row>
@@ -5443,13 +5736,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5" style="19" customWidth="1"/>
     <col min="2" max="2" width="14.625" style="19" customWidth="1"/>
@@ -5458,7 +5751,7 @@
     <col min="5" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -5466,13 +5759,13 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -5486,7 +5779,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24">
         <v>1</v>
       </c>
@@ -5500,7 +5793,7 @@
         <v>41176</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.5">
+    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="24">
         <v>2</v>
       </c>
@@ -5514,7 +5807,7 @@
         <v>41679</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24">
         <v>3</v>
       </c>
@@ -5528,7 +5821,7 @@
         <v>42136</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="24">
         <v>4</v>
       </c>
@@ -5542,7 +5835,7 @@
         <v>42293</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26">
         <v>5</v>
       </c>
@@ -5556,7 +5849,7 @@
         <v>42312</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26">
         <v>6</v>
       </c>
@@ -5570,7 +5863,7 @@
         <v>42430</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -5584,7 +5877,7 @@
         <v>43026</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -5598,7 +5891,7 @@
         <v>43142</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -5612,7 +5905,7 @@
         <v>43397</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="82">
         <v>10</v>
       </c>
@@ -5626,7 +5919,7 @@
         <v>43761</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="82">
         <v>11</v>
       </c>
@@ -5638,6 +5931,20 @@
       </c>
       <c r="D14" s="104">
         <v>44329</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="82">
+        <v>12</v>
+      </c>
+      <c r="B15" s="82" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="103" t="s">
+        <v>126</v>
+      </c>
+      <c r="D15" s="104">
+        <v>44698</v>
       </c>
     </row>
   </sheetData>

</xml_diff>